<commit_message>
adding case checkExportToCSVApplyScale and checkExportToCSVNoScale; update function applyScaleRadio to AbstractPage; adding return Boolean for function selectImportMode
</commit_message>
<xml_diff>
--- a/trump_scenariosTrainer.xlsx
+++ b/trump_scenariosTrainer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\APAutomation\scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MavenProject\trump\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -250,12 +250,12 @@
 used in "retrieve multiple group"</t>
   </si>
   <si>
+    <t>value is Y or N.
+used in "Create From Excel"and select some form-&gt;"Adjustments"-&gt;"Import adjustments", after select file, select Scaled or No Scale.</t>
+  </si>
+  <si>
     <t>value is override or additive.
-Used in import file, override means selected "Replace existing return(if any), additive means selected "Add to existing value(Numeric cells only)</t>
-  </si>
-  <si>
-    <t>value is Y or N.
-used in Create From Excel, after select file, select Scaled or No Scale.</t>
+Used in import file(select some form-&gt;"Adjustments"-&gt;"Import adjustments"), override means selected "Replace existing return(if any), additive means selected "Add to existing value(Numeric cells only)</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,10 +865,10 @@
         <v>73</v>
       </c>
       <c r="AC2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>